<commit_message>
updating solutions for day 3b
</commit_message>
<xml_diff>
--- a/d3.xlsx
+++ b/d3.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twon002/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twon002/Code/advent/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="d3a" sheetId="1" r:id="rId1"/>
+    <sheet name="d3b" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -66,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,8 +107,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,8 +140,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -141,13 +155,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -157,10 +225,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1293,4 +1369,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="7">
+        <v>369601</v>
+      </c>
+      <c r="C5" s="7">
+        <v>363010</v>
+      </c>
+      <c r="D5" s="7">
+        <v>349975</v>
+      </c>
+      <c r="E5" s="7">
+        <v>330785</v>
+      </c>
+      <c r="F5" s="7">
+        <v>312453</v>
+      </c>
+      <c r="G5" s="7">
+        <v>295229</v>
+      </c>
+      <c r="H5" s="7">
+        <v>279138</v>
+      </c>
+      <c r="I5" s="7">
+        <v>266330</v>
+      </c>
+      <c r="J5" s="7">
+        <v>130654</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7">
+        <v>6591</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6444</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6155</v>
+      </c>
+      <c r="F6" s="7">
+        <v>5733</v>
+      </c>
+      <c r="G6" s="7">
+        <v>5336</v>
+      </c>
+      <c r="H6" s="7">
+        <v>5022</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2450</v>
+      </c>
+      <c r="J6" s="7">
+        <v>128204</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7">
+        <v>13486</v>
+      </c>
+      <c r="D7" s="8">
+        <v>147</v>
+      </c>
+      <c r="E7" s="9">
+        <v>142</v>
+      </c>
+      <c r="F7" s="9">
+        <v>133</v>
+      </c>
+      <c r="G7" s="9">
+        <v>122</v>
+      </c>
+      <c r="H7" s="9">
+        <v>59</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2391</v>
+      </c>
+      <c r="J7" s="7">
+        <v>123363</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
+        <v>14267</v>
+      </c>
+      <c r="D8" s="10">
+        <v>304</v>
+      </c>
+      <c r="E8" s="11">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11">
+        <v>4</v>
+      </c>
+      <c r="G8" s="11">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11">
+        <v>57</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2275</v>
+      </c>
+      <c r="J8" s="7">
+        <v>116247</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7">
+        <v>15252</v>
+      </c>
+      <c r="D9" s="10">
+        <v>330</v>
+      </c>
+      <c r="E9" s="11">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>54</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2105</v>
+      </c>
+      <c r="J9" s="7">
+        <v>109476</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7">
+        <v>16295</v>
+      </c>
+      <c r="D10" s="10">
+        <v>351</v>
+      </c>
+      <c r="E10" s="11">
+        <v>11</v>
+      </c>
+      <c r="F10" s="11">
+        <v>23</v>
+      </c>
+      <c r="G10" s="11">
+        <v>25</v>
+      </c>
+      <c r="H10" s="11">
+        <v>26</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1968</v>
+      </c>
+      <c r="J10" s="7">
+        <v>103128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
+        <v>17008</v>
+      </c>
+      <c r="D11" s="12">
+        <v>362</v>
+      </c>
+      <c r="E11" s="12">
+        <v>747</v>
+      </c>
+      <c r="F11" s="12">
+        <v>806</v>
+      </c>
+      <c r="G11" s="7">
+        <v>880</v>
+      </c>
+      <c r="H11" s="7">
+        <v>931</v>
+      </c>
+      <c r="I11" s="7">
+        <v>957</v>
+      </c>
+      <c r="J11" s="7">
+        <v>98098</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7">
+        <v>17370</v>
+      </c>
+      <c r="D12" s="7">
+        <v>35487</v>
+      </c>
+      <c r="E12" s="7">
+        <v>37402</v>
+      </c>
+      <c r="F12" s="7">
+        <v>39835</v>
+      </c>
+      <c r="G12" s="7">
+        <v>42452</v>
+      </c>
+      <c r="H12" s="7">
+        <v>45220</v>
+      </c>
+      <c r="I12" s="7">
+        <v>47108</v>
+      </c>
+      <c r="J12" s="7">
+        <v>48065</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>